<commit_message>
Revert "Revert "Tilstandsdiagram færdig""
This reverts commit 29c127d962fe0e3671177b63297bd6d452a597bc.
</commit_message>
<xml_diff>
--- a/System udvikling/Hændelsestabel.xlsx
+++ b/System udvikling/Hændelsestabel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Hændelser/Klasser</t>
   </si>
@@ -63,15 +63,6 @@
     <t>KontoudtogLinje</t>
   </si>
   <si>
-    <t>Faktura er ikke betalt indenfor betalingsfrist</t>
-  </si>
-  <si>
-    <t>Betaling for faktura modtaget indenfor betalingsfrist</t>
-  </si>
-  <si>
-    <t>Ordre er sendt</t>
-  </si>
-  <si>
     <t>Ordre er produceret</t>
   </si>
   <si>
@@ -109,6 +100,30 @@
   </si>
   <si>
     <t>Vare indgår i ordre</t>
+  </si>
+  <si>
+    <t>Ordre rettes</t>
+  </si>
+  <si>
+    <t>Ordre er leveret</t>
+  </si>
+  <si>
+    <t>Ordre laves til faktura</t>
+  </si>
+  <si>
+    <t>faktura sendes</t>
+  </si>
+  <si>
+    <t>faktura annulleres</t>
+  </si>
+  <si>
+    <t>faktura rettes</t>
+  </si>
+  <si>
+    <t>faktura betalt</t>
+  </si>
+  <si>
+    <t>Rykker sendes</t>
   </si>
 </sst>
 </file>
@@ -490,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -526,7 +541,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -567,7 +582,7 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -587,7 +602,7 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -607,7 +622,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -627,7 +642,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -647,7 +662,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -667,7 +682,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="3"/>
@@ -687,7 +702,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="3"/>
@@ -707,7 +722,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="3"/>
@@ -727,7 +742,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="3"/>
@@ -747,7 +762,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
@@ -767,14 +782,14 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="B12" s="4"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -787,7 +802,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -807,7 +822,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -827,7 +842,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -847,7 +862,7 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -859,11 +874,111 @@
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
-      <c r="L16" s="4"/>
+      <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>